<commit_message>
updating all my codes
</commit_message>
<xml_diff>
--- a/Surface_Area/Wax_Dipping_Curve_091522.xlsx
+++ b/Surface_Area/Wax_Dipping_Curve_091522.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayrlindsay/Desktop/TO DO : ORGANIZE/Wax dipping/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayrlindsay/Desktop/GITHUB/TLPR21/Surface_Area/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB582B90-ABED-C647-82B0-CBA42D9B5928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF9C4F7-98D0-A242-B0F0-E852737F7931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="5360" windowWidth="16340" windowHeight="14120" xr2:uid="{2F1CA768-4583-1C44-87F9-52AEB5B7B3F0}"/>
+    <workbookView xWindow="5040" yWindow="680" windowWidth="16340" windowHeight="14120" xr2:uid="{2F1CA768-4583-1C44-87F9-52AEB5B7B3F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
-    <t>Colony ID</t>
-  </si>
-  <si>
     <t>Standard1</t>
   </si>
   <si>
@@ -77,24 +74,6 @@
     <t xml:space="preserve">Standard12 </t>
   </si>
   <si>
-    <t>Sample diameter</t>
-  </si>
-  <si>
-    <t>Weight1</t>
-  </si>
-  <si>
-    <t>Wax_Weight</t>
-  </si>
-  <si>
-    <t>Radius</t>
-  </si>
-  <si>
-    <t>Surface_Area</t>
-  </si>
-  <si>
-    <t>Difference</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
@@ -105,6 +84,27 @@
   </si>
   <si>
     <t>*must be more than 0.9</t>
+  </si>
+  <si>
+    <t>colony_id</t>
+  </si>
+  <si>
+    <t>diameter</t>
+  </si>
+  <si>
+    <t>weight1</t>
+  </si>
+  <si>
+    <t>wax_weight</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
+    <t>surface_area</t>
+  </si>
+  <si>
+    <t>difference</t>
   </si>
 </sst>
 </file>
@@ -189,7 +189,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Difference</c:v>
+                  <c:v>difference</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1550,8 +1550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83D30A9-8ED2-524C-BD85-0F407104989A}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1560,34 +1560,40 @@
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>2.86</v>
@@ -1613,7 +1619,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>2.9</v>
@@ -1637,18 +1643,18 @@
         <v>0.85890000000000022</v>
       </c>
       <c r="O3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="P3">
         <v>0.94979999999999998</v>
       </c>
       <c r="Q3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>2.41</v>
@@ -1672,7 +1678,7 @@
         <v>0.70249999999999968</v>
       </c>
       <c r="O4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="P4">
         <v>3.5900000000000001E-2</v>
@@ -1680,7 +1686,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>2.44</v>
@@ -1704,7 +1710,7 @@
         <v>0.45610000000000017</v>
       </c>
       <c r="O5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="P5">
         <v>-5.9499999999999997E-2</v>
@@ -1712,7 +1718,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>1.93</v>
@@ -1738,7 +1744,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>1.96</v>
@@ -1764,7 +1770,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>1.5</v>
@@ -1790,7 +1796,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
         <v>1.52</v>
@@ -1816,7 +1822,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>1.1399999999999999</v>
@@ -1842,7 +1848,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>1.17</v>
@@ -1868,7 +1874,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>0.97</v>
@@ -1894,7 +1900,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>0.94</v>

</xml_diff>